<commit_message>
feedback form updated and patch to warn rather than fail when feedback form and tracker sector type slightly disagree
</commit_message>
<xml_diff>
--- a/feedback_forms/current_versions/energy_operator_feedback_v003.xlsx
+++ b/feedback_forms/current_versions/energy_operator_feedback_v003.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\one_drive\code\pycharm\feedback_portal\feedback_forms\current_versions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\one_drive\OneDriveLinks\RD Satellite Project - Operator Notification Materials for Review\spreadsheets\xl_workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C623C966-276C-4D6F-BE5B-C1BF9F1BBEB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA342922-C8B5-46FA-B288-345579CA7358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5447" yWindow="1447" windowWidth="19200" windowHeight="11760" xr2:uid="{AD2102A5-37B4-471F-BCEC-083B2F5B9811}"/>
+    <workbookView xWindow="2980" yWindow="333" windowWidth="21293" windowHeight="13840" xr2:uid="{AD2102A5-37B4-471F-BCEC-083B2F5B9811}"/>
   </bookViews>
   <sheets>
     <sheet name="Feedback Form" sheetId="5" r:id="rId1"/>
@@ -5406,9 +5406,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A2:R35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:R35"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
@@ -5943,6 +5941,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000E9A34E7C7C736409D4BDE6375CCC276" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0cf521a6d855790dbe6a6d894ff439cd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32" xmlns:ns3="e20ceb87-0d79-402a-b4b9-75d78589c76d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a45aa6d812898c4b0f52b4c3685679ce" ns2:_="" ns3:_="">
     <xsd:import namespace="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32"/>
@@ -6177,15 +6184,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{368BC477-8FFD-4C56-8224-F3CCFEFBFA36}">
   <ds:schemaRefs>
@@ -6198,6 +6196,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{393EEAE4-A9A0-45DD-A8E7-CAAABB0BE8BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{533C6BB5-3BBA-46E5-A63A-38A55F0F20F9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6214,12 +6220,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{393EEAE4-A9A0-45DD-A8E7-CAAABB0BE8BF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updating parse for aliased schemas
</commit_message>
<xml_diff>
--- a/feedback_forms/current_versions/energy_operator_feedback_v003.xlsx
+++ b/feedback_forms/current_versions/energy_operator_feedback_v003.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\local\cursor\feedback_portal\feedback_forms\current_versions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tony_local\pycharm\feedback_portal\feedback_forms\current_versions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2279E71-D0EC-4470-9C48-59B1D9F35A5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A878B4-A0A3-4B7A-8A89-1F7FC3B7D496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4877" yWindow="1637" windowWidth="23897" windowHeight="15892" activeTab="4" xr2:uid="{AD2102A5-37B4-471F-BCEC-083B2F5B9811}"/>
+    <workbookView xWindow="4193" yWindow="2087" windowWidth="19200" windowHeight="11386" activeTab="4" xr2:uid="{AD2102A5-37B4-471F-BCEC-083B2F5B9811}"/>
   </bookViews>
   <sheets>
     <sheet name="Feedback Form" sheetId="5" r:id="rId1"/>
@@ -2479,19 +2479,19 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="4.15234375" customWidth="1"/>
-    <col min="2" max="2" width="65.69140625" customWidth="1"/>
-    <col min="3" max="3" width="4.69140625" customWidth="1"/>
-    <col min="4" max="4" width="65.69140625" customWidth="1"/>
-    <col min="5" max="5" width="4.15234375" customWidth="1"/>
-    <col min="6" max="6" width="5.69140625" style="22" customWidth="1"/>
-    <col min="7" max="7" width="28.53515625" customWidth="1"/>
-    <col min="8" max="8" width="22.15234375" customWidth="1"/>
+    <col min="1" max="1" width="4.17578125" customWidth="1"/>
+    <col min="2" max="2" width="65.703125" customWidth="1"/>
+    <col min="3" max="3" width="4.703125" customWidth="1"/>
+    <col min="4" max="4" width="65.703125" customWidth="1"/>
+    <col min="5" max="5" width="4.17578125" customWidth="1"/>
+    <col min="6" max="6" width="5.703125" style="22" customWidth="1"/>
+    <col min="7" max="7" width="28.52734375" customWidth="1"/>
+    <col min="8" max="8" width="22.17578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:33" s="23" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:33" s="23" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
       <c r="D1" s="21"/>
@@ -2527,7 +2527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:33" s="23" customFormat="1" ht="51" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:33" s="23" customFormat="1" ht="51" x14ac:dyDescent="0.5">
       <c r="B2" s="24" t="s">
         <v>1</v>
       </c>
@@ -2536,7 +2536,7 @@
       <c r="E2" s="24"/>
       <c r="F2" s="40"/>
     </row>
-    <row r="3" spans="2:33" s="23" customFormat="1" ht="51" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:33" s="23" customFormat="1" ht="51" x14ac:dyDescent="0.5">
       <c r="B3" s="24" t="s">
         <v>156</v>
       </c>
@@ -2545,14 +2545,14 @@
       <c r="E3" s="24"/>
       <c r="F3" s="40"/>
     </row>
-    <row r="4" spans="2:33" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:33" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
       <c r="D4" s="25"/>
       <c r="E4" s="26"/>
       <c r="F4" s="40"/>
     </row>
-    <row r="5" spans="2:33" s="23" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:33" s="23" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
       <c r="D5" s="21"/>
@@ -2588,7 +2588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:33" s="27" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:33" s="27" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="41"/>
       <c r="C6" s="41"/>
       <c r="D6" s="41"/>
@@ -2622,7 +2622,7 @@
       <c r="AF6" s="42"/>
       <c r="AG6" s="42"/>
     </row>
-    <row r="7" spans="2:33" s="23" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:33" s="23" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B7" s="21"/>
       <c r="C7" s="21"/>
       <c r="D7" s="21"/>
@@ -2658,7 +2658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B8" s="52" t="s">
         <v>135</v>
       </c>
@@ -2667,7 +2667,7 @@
       <c r="E8" s="31"/>
       <c r="F8" s="40"/>
     </row>
-    <row r="9" spans="2:33" s="30" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:33" s="30" customFormat="1" ht="20.2" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B9" s="54" t="s">
         <v>137</v>
       </c>
@@ -2676,7 +2676,7 @@
       <c r="E9" s="31"/>
       <c r="F9" s="40"/>
     </row>
-    <row r="10" spans="2:33" s="30" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:33" s="30" customFormat="1" ht="20.2" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B10" s="53" t="s">
         <v>136</v>
       </c>
@@ -2685,7 +2685,7 @@
       <c r="E10" s="31"/>
       <c r="F10" s="40"/>
     </row>
-    <row r="11" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B11" s="52" t="s">
         <v>138</v>
       </c>
@@ -2694,7 +2694,7 @@
       <c r="E11" s="31"/>
       <c r="F11" s="40"/>
     </row>
-    <row r="12" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B12" s="52" t="s">
         <v>139</v>
       </c>
@@ -2703,7 +2703,7 @@
       <c r="E12" s="31"/>
       <c r="F12" s="40"/>
     </row>
-    <row r="13" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B13" s="55" t="s">
         <v>140</v>
       </c>
@@ -2739,7 +2739,7 @@
       <c r="AF13" s="29"/>
       <c r="AG13" s="29"/>
     </row>
-    <row r="14" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B14" s="57" t="s">
         <v>164</v>
       </c>
@@ -2775,7 +2775,7 @@
       <c r="AF14" s="29"/>
       <c r="AG14" s="29"/>
     </row>
-    <row r="15" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B15" s="58" t="s">
         <v>165</v>
       </c>
@@ -2784,7 +2784,7 @@
       <c r="E15" s="31"/>
       <c r="F15" s="40"/>
     </row>
-    <row r="16" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B16" s="56" t="s">
         <v>141</v>
       </c>
@@ -2793,7 +2793,7 @@
       <c r="E16" s="31"/>
       <c r="F16" s="40"/>
     </row>
-    <row r="17" spans="2:33" s="23" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:33" s="23" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B17" s="21"/>
       <c r="C17" s="21"/>
       <c r="D17" s="21"/>
@@ -2829,7 +2829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:33" s="32" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:33" s="32" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B18" s="41"/>
       <c r="C18" s="41"/>
       <c r="D18" s="41"/>
@@ -2863,7 +2863,7 @@
       <c r="AF18" s="44"/>
       <c r="AG18" s="44"/>
     </row>
-    <row r="19" spans="2:33" s="23" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:33" s="23" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B19" s="21"/>
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
@@ -2899,7 +2899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:33" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:33" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B20" s="50" t="s">
         <v>128</v>
       </c>
@@ -2910,7 +2910,7 @@
       <c r="E20" s="40"/>
       <c r="F20" s="40"/>
     </row>
-    <row r="21" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B21" s="50" t="s">
         <v>129</v>
       </c>
@@ -2921,7 +2921,7 @@
       <c r="E21" s="40"/>
       <c r="F21" s="40"/>
     </row>
-    <row r="22" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B22" s="50" t="s">
         <v>130</v>
       </c>
@@ -2932,7 +2932,7 @@
       <c r="E22" s="40"/>
       <c r="F22" s="40"/>
     </row>
-    <row r="23" spans="2:33" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:33" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B23" s="50" t="s">
         <v>131</v>
       </c>
@@ -2943,7 +2943,7 @@
       <c r="E23" s="40"/>
       <c r="F23" s="40"/>
     </row>
-    <row r="24" spans="2:33" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:33" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B24" s="50" t="s">
         <v>132</v>
       </c>
@@ -2954,7 +2954,7 @@
       <c r="E24" s="40"/>
       <c r="F24" s="40"/>
     </row>
-    <row r="25" spans="2:33" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:33" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B25" s="50" t="s">
         <v>133</v>
       </c>
@@ -2965,7 +2965,7 @@
       <c r="E25" s="40"/>
       <c r="F25" s="40"/>
     </row>
-    <row r="26" spans="2:33" s="23" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:33" s="23" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B26" s="21"/>
       <c r="C26" s="21"/>
       <c r="D26" s="21"/>
@@ -3001,7 +3001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:33" s="27" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:33" s="27" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B27" s="41"/>
       <c r="C27" s="41"/>
       <c r="D27" s="41"/>
@@ -3035,7 +3035,7 @@
       <c r="AF27" s="42"/>
       <c r="AG27" s="42"/>
     </row>
-    <row r="28" spans="2:33" s="23" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:33" s="23" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B28" s="21"/>
       <c r="C28" s="21"/>
       <c r="D28" s="21"/>
@@ -3071,7 +3071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:33" s="10" customFormat="1" ht="15.45" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:33" s="10" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
       <c r="B29" s="51" t="s">
         <v>134</v>
       </c>
@@ -3082,7 +3082,7 @@
       <c r="E29" s="47"/>
       <c r="F29" s="40"/>
     </row>
-    <row r="30" spans="2:33" s="10" customFormat="1" ht="15.45" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:33" s="10" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
       <c r="B30" s="59" t="s">
         <v>166</v>
       </c>
@@ -3093,7 +3093,7 @@
       <c r="E30" s="47"/>
       <c r="F30" s="40"/>
     </row>
-    <row r="31" spans="2:33" s="10" customFormat="1" ht="15.45" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:33" s="10" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
       <c r="B31" s="59" t="s">
         <v>167</v>
       </c>
@@ -3104,7 +3104,7 @@
       <c r="E31" s="47"/>
       <c r="F31" s="40"/>
     </row>
-    <row r="32" spans="2:33" s="10" customFormat="1" ht="15.45" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:33" s="10" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
       <c r="B32" s="59" t="s">
         <v>168</v>
       </c>
@@ -3115,7 +3115,7 @@
       <c r="E32" s="47"/>
       <c r="F32" s="40"/>
     </row>
-    <row r="33" spans="2:33" s="23" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:33" s="23" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
       <c r="D33" s="21"/>
@@ -3151,7 +3151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:33" s="27" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:33" s="27" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B34" s="41"/>
       <c r="C34" s="41"/>
       <c r="D34" s="41"/>
@@ -3185,7 +3185,7 @@
       <c r="AF34" s="42"/>
       <c r="AG34" s="42"/>
     </row>
-    <row r="35" spans="2:33" s="23" customFormat="1" ht="15.45" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:33" s="23" customFormat="1" ht="15.35" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B35" s="21"/>
       <c r="C35" s="21"/>
       <c r="D35" s="21"/>
@@ -3221,7 +3221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:33" s="15" customFormat="1" ht="50.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:33" s="15" customFormat="1" ht="50.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B36" s="59" t="s">
         <v>169</v>
       </c>
@@ -3232,7 +3232,7 @@
       <c r="E36" s="34"/>
       <c r="F36" s="40"/>
     </row>
-    <row r="37" spans="2:33" s="15" customFormat="1" ht="31.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:33" s="15" customFormat="1" ht="31" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B37" s="59" t="s">
         <v>170</v>
       </c>
@@ -3243,7 +3243,7 @@
       <c r="E37" s="34"/>
       <c r="F37" s="40"/>
     </row>
-    <row r="38" spans="2:33" s="15" customFormat="1" ht="50.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:33" s="15" customFormat="1" ht="50.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B38" s="59" t="s">
         <v>171</v>
       </c>
@@ -3254,7 +3254,7 @@
       <c r="E38" s="34"/>
       <c r="F38" s="40"/>
     </row>
-    <row r="39" spans="2:33" s="15" customFormat="1" ht="50.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:33" s="15" customFormat="1" ht="50.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B39" s="59" t="s">
         <v>172</v>
       </c>
@@ -3265,7 +3265,7 @@
       <c r="E39" s="34"/>
       <c r="F39" s="40"/>
     </row>
-    <row r="40" spans="2:33" s="15" customFormat="1" ht="31.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:33" s="15" customFormat="1" ht="31" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B40" s="59" t="s">
         <v>173</v>
       </c>
@@ -3276,7 +3276,7 @@
       <c r="E40" s="34"/>
       <c r="F40" s="40"/>
     </row>
-    <row r="41" spans="2:33" s="15" customFormat="1" ht="50.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:33" s="15" customFormat="1" ht="50.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B41" s="59" t="s">
         <v>174</v>
       </c>
@@ -3287,7 +3287,7 @@
       <c r="E41" s="34"/>
       <c r="F41" s="40"/>
     </row>
-    <row r="42" spans="2:33" s="15" customFormat="1" ht="30.9" thickTop="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="2:33" s="15" customFormat="1" ht="30.7" thickTop="1" x14ac:dyDescent="0.5">
       <c r="B42" s="59" t="s">
         <v>175</v>
       </c>
@@ -3298,7 +3298,7 @@
       <c r="E42" s="34"/>
       <c r="F42" s="40"/>
     </row>
-    <row r="43" spans="2:33" s="15" customFormat="1" ht="45.45" x14ac:dyDescent="0.4">
+    <row r="43" spans="2:33" s="15" customFormat="1" ht="45.35" x14ac:dyDescent="0.5">
       <c r="B43" s="33" t="s">
         <v>176</v>
       </c>
@@ -3309,7 +3309,7 @@
       <c r="E43" s="40"/>
       <c r="F43" s="40"/>
     </row>
-    <row r="44" spans="2:33" s="15" customFormat="1" ht="45.45" x14ac:dyDescent="0.4">
+    <row r="44" spans="2:33" s="15" customFormat="1" ht="45.35" x14ac:dyDescent="0.5">
       <c r="B44" s="59" t="s">
         <v>177</v>
       </c>
@@ -3320,7 +3320,7 @@
       <c r="E44" s="40"/>
       <c r="F44" s="40"/>
     </row>
-    <row r="45" spans="2:33" s="23" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="2:33" s="23" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B45" s="21"/>
       <c r="C45" s="21"/>
       <c r="D45" s="21"/>
@@ -3356,7 +3356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:33" s="27" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:33" s="27" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B46" s="41"/>
       <c r="C46" s="41"/>
       <c r="D46" s="41"/>
@@ -3390,7 +3390,7 @@
       <c r="AF46" s="42"/>
       <c r="AG46" s="42"/>
     </row>
-    <row r="47" spans="2:33" s="23" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="2:33" s="23" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B47" s="21"/>
       <c r="C47" s="21"/>
       <c r="D47" s="21"/>
@@ -3426,7 +3426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:33" s="15" customFormat="1" ht="15.45" x14ac:dyDescent="0.4">
+    <row r="48" spans="2:33" s="15" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
       <c r="B48" s="59" t="s">
         <v>185</v>
       </c>
@@ -3437,7 +3437,7 @@
       <c r="E48" s="36"/>
       <c r="F48" s="40"/>
     </row>
-    <row r="49" spans="2:33" s="15" customFormat="1" ht="30.45" x14ac:dyDescent="0.4">
+    <row r="49" spans="2:33" s="15" customFormat="1" ht="30.35" x14ac:dyDescent="0.5">
       <c r="B49" s="59" t="s">
         <v>186</v>
       </c>
@@ -3448,7 +3448,7 @@
       <c r="E49" s="40"/>
       <c r="F49" s="40"/>
     </row>
-    <row r="50" spans="2:33" s="15" customFormat="1" ht="15.45" x14ac:dyDescent="0.4">
+    <row r="50" spans="2:33" s="15" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
       <c r="B50" s="59" t="s">
         <v>180</v>
       </c>
@@ -3459,7 +3459,7 @@
       <c r="E50" s="40"/>
       <c r="F50" s="40"/>
     </row>
-    <row r="51" spans="2:33" s="15" customFormat="1" ht="15.45" x14ac:dyDescent="0.4">
+    <row r="51" spans="2:33" s="15" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
       <c r="B51" s="59" t="s">
         <v>181</v>
       </c>
@@ -3470,7 +3470,7 @@
       <c r="E51" s="40"/>
       <c r="F51" s="40"/>
     </row>
-    <row r="52" spans="2:33" s="15" customFormat="1" ht="15.45" x14ac:dyDescent="0.4">
+    <row r="52" spans="2:33" s="15" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
       <c r="B52" s="33" t="s">
         <v>182</v>
       </c>
@@ -3481,7 +3481,7 @@
       <c r="E52" s="40"/>
       <c r="F52" s="40"/>
     </row>
-    <row r="53" spans="2:33" s="23" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="2:33" s="23" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B53" s="21"/>
       <c r="C53" s="21"/>
       <c r="D53" s="21"/>
@@ -3517,10 +3517,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:33" ht="40" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="2:33" ht="40" customHeight="1" x14ac:dyDescent="0.5">
       <c r="F54" s="40"/>
     </row>
-    <row r="56" spans="2:33" s="15" customFormat="1" ht="15.45" x14ac:dyDescent="0.4">
+    <row r="56" spans="2:33" s="15" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
       <c r="B56" s="33" t="s">
         <v>184</v>
       </c>
@@ -3568,25 +3568,25 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="3.69140625" customWidth="1"/>
-    <col min="2" max="2" width="10.69140625" customWidth="1"/>
-    <col min="3" max="3" width="45.69140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.3828125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.53515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.703125" customWidth="1"/>
+    <col min="2" max="2" width="10.703125" customWidth="1"/>
+    <col min="3" max="3" width="45.703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.3515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.52734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="45.69140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="45.703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" s="13" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:18" s="13" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="B2" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="14"/>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.5">
       <c r="G3" s="17"/>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
@@ -3600,7 +3600,7 @@
       <c r="Q3" s="11"/>
       <c r="R3" s="11"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -3608,15 +3608,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.5">
       <c r="B10" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.5">
       <c r="B11" s="7"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.5">
       <c r="B12" t="s">
         <v>13</v>
       </c>
@@ -3624,7 +3624,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:18" s="10" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B13" s="10" t="s">
         <v>15</v>
       </c>
@@ -3634,7 +3634,7 @@
       <c r="D13" s="16"/>
       <c r="G13" s="15"/>
     </row>
-    <row r="14" spans="1:18" s="10" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:18" s="10" customFormat="1" ht="43" x14ac:dyDescent="0.5">
       <c r="B14" s="10" t="s">
         <v>17</v>
       </c>
@@ -3644,7 +3644,7 @@
       <c r="D14" s="16"/>
       <c r="G14" s="15"/>
     </row>
-    <row r="15" spans="1:18" s="10" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:18" s="10" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B15" s="15" t="s">
         <v>19</v>
       </c>
@@ -3654,7 +3654,7 @@
       <c r="D15" s="16"/>
       <c r="G15" s="15"/>
     </row>
-    <row r="16" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B16" s="10" t="s">
         <v>21</v>
       </c>
@@ -3664,7 +3664,7 @@
       <c r="D16" s="16"/>
       <c r="G16" s="15"/>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.5">
       <c r="B18" s="7" t="s">
         <v>23</v>
       </c>
@@ -3681,7 +3681,7 @@
       <c r="Q18" s="11"/>
       <c r="R18" s="11"/>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:18" x14ac:dyDescent="0.5">
       <c r="G19" s="17"/>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
@@ -3695,7 +3695,7 @@
       <c r="Q19" s="11"/>
       <c r="R19" s="11"/>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:18" x14ac:dyDescent="0.5">
       <c r="B20" t="s">
         <v>24</v>
       </c>
@@ -3726,7 +3726,7 @@
       <c r="Q20" s="11"/>
       <c r="R20" s="11"/>
     </row>
-    <row r="21" spans="2:18" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:18" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B21" s="10">
         <v>1</v>
       </c>
@@ -3745,7 +3745,7 @@
       </c>
       <c r="G21" s="15"/>
     </row>
-    <row r="22" spans="2:18" s="10" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:18" s="10" customFormat="1" ht="100.35" x14ac:dyDescent="0.5">
       <c r="B22" s="10">
         <v>2</v>
       </c>
@@ -3766,7 +3766,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="23" spans="2:18" s="10" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:18" s="10" customFormat="1" ht="43" x14ac:dyDescent="0.5">
       <c r="B23" s="10">
         <v>3</v>
       </c>
@@ -3785,7 +3785,7 @@
       </c>
       <c r="G23" s="15"/>
     </row>
-    <row r="24" spans="2:18" s="10" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:18" s="10" customFormat="1" ht="43" x14ac:dyDescent="0.5">
       <c r="B24" s="10">
         <v>4</v>
       </c>
@@ -3806,7 +3806,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="25" spans="2:18" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:18" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B25" s="10">
         <v>5</v>
       </c>
@@ -3814,7 +3814,7 @@
       <c r="D25" s="16"/>
       <c r="G25" s="15"/>
     </row>
-    <row r="26" spans="2:18" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:18" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B26" s="10">
         <v>6</v>
       </c>
@@ -3822,7 +3822,7 @@
       <c r="D26" s="16"/>
       <c r="G26" s="15"/>
     </row>
-    <row r="27" spans="2:18" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:18" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B27" s="10">
         <v>7</v>
       </c>
@@ -3830,7 +3830,7 @@
       <c r="D27" s="16"/>
       <c r="G27" s="15"/>
     </row>
-    <row r="28" spans="2:18" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:18" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B28" s="10">
         <v>8</v>
       </c>
@@ -3838,7 +3838,7 @@
       <c r="D28" s="16"/>
       <c r="G28" s="15"/>
     </row>
-    <row r="29" spans="2:18" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:18" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B29" s="10">
         <v>9</v>
       </c>
@@ -3846,7 +3846,7 @@
       <c r="D29" s="16"/>
       <c r="G29" s="15"/>
     </row>
-    <row r="30" spans="2:18" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:18" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B30" s="10">
         <v>10</v>
       </c>
@@ -3854,7 +3854,7 @@
       <c r="D30" s="16"/>
       <c r="G30" s="15"/>
     </row>
-    <row r="31" spans="2:18" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:18" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B31" s="10">
         <v>11</v>
       </c>
@@ -3862,7 +3862,7 @@
       <c r="D31" s="16"/>
       <c r="G31" s="15"/>
     </row>
-    <row r="32" spans="2:18" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:18" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B32" s="10">
         <v>12</v>
       </c>
@@ -3870,7 +3870,7 @@
       <c r="D32" s="16"/>
       <c r="G32" s="15"/>
     </row>
-    <row r="33" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B33" s="10">
         <v>13</v>
       </c>
@@ -3878,7 +3878,7 @@
       <c r="D33" s="16"/>
       <c r="G33" s="15"/>
     </row>
-    <row r="34" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B34" s="10">
         <v>14</v>
       </c>
@@ -3886,7 +3886,7 @@
       <c r="D34" s="16"/>
       <c r="G34" s="15"/>
     </row>
-    <row r="35" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B35" s="10">
         <v>15</v>
       </c>
@@ -3894,7 +3894,7 @@
       <c r="D35" s="16"/>
       <c r="G35" s="15"/>
     </row>
-    <row r="36" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B36" s="10">
         <v>16</v>
       </c>
@@ -3902,7 +3902,7 @@
       <c r="D36" s="16"/>
       <c r="G36" s="15"/>
     </row>
-    <row r="37" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B37" s="10">
         <v>17</v>
       </c>
@@ -3910,7 +3910,7 @@
       <c r="D37" s="16"/>
       <c r="G37" s="15"/>
     </row>
-    <row r="38" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B38" s="10">
         <v>18</v>
       </c>
@@ -3918,7 +3918,7 @@
       <c r="D38" s="16"/>
       <c r="G38" s="15"/>
     </row>
-    <row r="39" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B39" s="10">
         <v>19</v>
       </c>
@@ -3926,7 +3926,7 @@
       <c r="D39" s="16"/>
       <c r="G39" s="15"/>
     </row>
-    <row r="40" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B40" s="10">
         <v>20</v>
       </c>
@@ -3934,7 +3934,7 @@
       <c r="D40" s="16"/>
       <c r="G40" s="15"/>
     </row>
-    <row r="41" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B41" s="10">
         <v>21</v>
       </c>
@@ -3942,7 +3942,7 @@
       <c r="D41" s="16"/>
       <c r="G41" s="15"/>
     </row>
-    <row r="42" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B42" s="10">
         <v>22</v>
       </c>
@@ -3950,7 +3950,7 @@
       <c r="D42" s="16"/>
       <c r="G42" s="15"/>
     </row>
-    <row r="43" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B43" s="10">
         <v>23</v>
       </c>
@@ -3958,7 +3958,7 @@
       <c r="D43" s="16"/>
       <c r="G43" s="15"/>
     </row>
-    <row r="44" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B44" s="10">
         <v>24</v>
       </c>
@@ -3966,7 +3966,7 @@
       <c r="D44" s="16"/>
       <c r="G44" s="15"/>
     </row>
-    <row r="45" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B45" s="10">
         <v>25</v>
       </c>
@@ -3974,7 +3974,7 @@
       <c r="D45" s="16"/>
       <c r="G45" s="15"/>
     </row>
-    <row r="46" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B46" s="10">
         <v>26</v>
       </c>
@@ -3982,7 +3982,7 @@
       <c r="D46" s="16"/>
       <c r="G46" s="15"/>
     </row>
-    <row r="47" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B47" s="10">
         <v>27</v>
       </c>
@@ -3990,7 +3990,7 @@
       <c r="D47" s="16"/>
       <c r="G47" s="15"/>
     </row>
-    <row r="48" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B48" s="10">
         <v>28</v>
       </c>
@@ -3998,7 +3998,7 @@
       <c r="D48" s="16"/>
       <c r="G48" s="15"/>
     </row>
-    <row r="49" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B49" s="10">
         <v>29</v>
       </c>
@@ -4006,47 +4006,47 @@
       <c r="D49" s="16"/>
       <c r="G49" s="15"/>
     </row>
-    <row r="50" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="C50" s="15"/>
       <c r="G50" s="15"/>
     </row>
-    <row r="51" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="C51" s="15"/>
       <c r="G51" s="15"/>
     </row>
-    <row r="52" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="C52" s="15"/>
       <c r="G52" s="15"/>
     </row>
-    <row r="53" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="C53" s="15"/>
       <c r="G53" s="15"/>
     </row>
-    <row r="54" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="C54" s="15"/>
       <c r="G54" s="15"/>
     </row>
-    <row r="55" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="C55" s="15"/>
       <c r="G55" s="15"/>
     </row>
-    <row r="56" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="C56" s="15"/>
       <c r="G56" s="15"/>
     </row>
-    <row r="57" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="C57" s="15"/>
       <c r="G57" s="15"/>
     </row>
-    <row r="58" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="C58" s="15"/>
       <c r="G58" s="15"/>
     </row>
-    <row r="59" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="C59" s="15"/>
       <c r="G59" s="15"/>
     </row>
-    <row r="60" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="60" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="C60" s="15"/>
       <c r="G60" s="15"/>
     </row>
@@ -4071,14 +4071,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="3.69140625" customWidth="1"/>
-    <col min="2" max="2" width="91.3046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="86.15234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.703125" customWidth="1"/>
+    <col min="2" max="2" width="91.29296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="86.17578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.5">
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
       <c r="H1" s="11"/>
@@ -4092,12 +4092,12 @@
       <c r="P1" s="11"/>
       <c r="Q1" s="11"/>
     </row>
-    <row r="2" spans="1:17" s="13" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:17" s="13" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="B2" s="13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.5">
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
@@ -4111,7 +4111,7 @@
       <c r="P3" s="11"/>
       <c r="Q3" s="11"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -4119,7 +4119,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -4127,7 +4127,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -4135,7 +4135,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.5">
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
@@ -4149,7 +4149,7 @@
       <c r="P8" s="11"/>
       <c r="Q8" s="11"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.5">
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
@@ -4163,7 +4163,7 @@
       <c r="P9" s="11"/>
       <c r="Q9" s="11"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.5">
       <c r="B10" s="7" t="s">
         <v>33</v>
       </c>
@@ -4180,7 +4180,7 @@
       <c r="P10" s="11"/>
       <c r="Q10" s="11"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.5">
       <c r="B11" s="7"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
@@ -4195,7 +4195,7 @@
       <c r="P11" s="11"/>
       <c r="Q11" s="11"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.5">
       <c r="B12" t="s">
         <v>8</v>
       </c>
@@ -4212,7 +4212,7 @@
       <c r="P12" s="11"/>
       <c r="Q12" s="11"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.5">
       <c r="B13" t="s">
         <v>7</v>
       </c>
@@ -4229,7 +4229,7 @@
       <c r="P13" s="11"/>
       <c r="Q13" s="11"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.5">
       <c r="B14" t="s">
         <v>34</v>
       </c>
@@ -4246,7 +4246,7 @@
       <c r="P14" s="11"/>
       <c r="Q14" s="11"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.5">
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
@@ -4260,7 +4260,7 @@
       <c r="P15" s="11"/>
       <c r="Q15" s="11"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.5">
       <c r="B16" s="7" t="s">
         <v>110</v>
       </c>
@@ -4277,7 +4277,7 @@
       <c r="P16" s="11"/>
       <c r="Q16" s="11"/>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.5">
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
       <c r="H17" s="11"/>
@@ -4291,7 +4291,7 @@
       <c r="P17" s="11"/>
       <c r="Q17" s="11"/>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B18" t="s">
         <v>8</v>
       </c>
@@ -4308,7 +4308,7 @@
       <c r="P18" s="11"/>
       <c r="Q18" s="11"/>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B19" t="s">
         <v>115</v>
       </c>
@@ -4325,7 +4325,7 @@
       <c r="P19" s="11"/>
       <c r="Q19" s="11"/>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B20" t="s">
         <v>35</v>
       </c>
@@ -4342,7 +4342,7 @@
       <c r="P20" s="11"/>
       <c r="Q20" s="11"/>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B21" t="s">
         <v>111</v>
       </c>
@@ -4359,7 +4359,7 @@
       <c r="P21" s="11"/>
       <c r="Q21" s="11"/>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B22" t="s">
         <v>112</v>
       </c>
@@ -4376,7 +4376,7 @@
       <c r="P22" s="11"/>
       <c r="Q22" s="11"/>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B23" t="s">
         <v>113</v>
       </c>
@@ -4393,7 +4393,7 @@
       <c r="P23" s="11"/>
       <c r="Q23" s="11"/>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B24" t="s">
         <v>114</v>
       </c>
@@ -4410,7 +4410,7 @@
       <c r="P24" s="11"/>
       <c r="Q24" s="11"/>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.5">
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
@@ -4424,7 +4424,7 @@
       <c r="P25" s="11"/>
       <c r="Q25" s="11"/>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B26" s="7" t="s">
         <v>118</v>
       </c>
@@ -4441,7 +4441,7 @@
       <c r="P26" s="11"/>
       <c r="Q26" s="11"/>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.5">
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
@@ -4455,7 +4455,7 @@
       <c r="P27" s="11"/>
       <c r="Q27" s="11"/>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B28" t="s">
         <v>8</v>
       </c>
@@ -4472,7 +4472,7 @@
       <c r="P28" s="11"/>
       <c r="Q28" s="11"/>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B29" t="s">
         <v>116</v>
       </c>
@@ -4489,7 +4489,7 @@
       <c r="P29" s="11"/>
       <c r="Q29" s="11"/>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B30" t="s">
         <v>35</v>
       </c>
@@ -4506,7 +4506,7 @@
       <c r="P30" s="11"/>
       <c r="Q30" s="11"/>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B31" t="s">
         <v>117</v>
       </c>
@@ -4523,7 +4523,7 @@
       <c r="P31" s="11"/>
       <c r="Q31" s="11"/>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B32" t="s">
         <v>111</v>
       </c>
@@ -4540,7 +4540,7 @@
       <c r="P32" s="11"/>
       <c r="Q32" s="11"/>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B33" t="s">
         <v>112</v>
       </c>
@@ -4557,7 +4557,7 @@
       <c r="P33" s="11"/>
       <c r="Q33" s="11"/>
     </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B34" t="s">
         <v>113</v>
       </c>
@@ -4574,7 +4574,7 @@
       <c r="P34" s="11"/>
       <c r="Q34" s="11"/>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B35" t="s">
         <v>114</v>
       </c>
@@ -4591,7 +4591,7 @@
       <c r="P35" s="11"/>
       <c r="Q35" s="11"/>
     </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.5">
       <c r="F36" s="11"/>
       <c r="G36" s="11"/>
       <c r="H36" s="11"/>
@@ -4605,7 +4605,7 @@
       <c r="P36" s="11"/>
       <c r="Q36" s="11"/>
     </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B37" s="7" t="s">
         <v>119</v>
       </c>
@@ -4622,7 +4622,7 @@
       <c r="P37" s="11"/>
       <c r="Q37" s="11"/>
     </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="38" spans="2:17" x14ac:dyDescent="0.5">
       <c r="F38" s="11"/>
       <c r="G38" s="11"/>
       <c r="H38" s="11"/>
@@ -4636,7 +4636,7 @@
       <c r="P38" s="11"/>
       <c r="Q38" s="11"/>
     </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="39" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B39" t="s">
         <v>8</v>
       </c>
@@ -4653,7 +4653,7 @@
       <c r="P39" s="11"/>
       <c r="Q39" s="11"/>
     </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="40" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B40" t="s">
         <v>116</v>
       </c>
@@ -4670,7 +4670,7 @@
       <c r="P40" s="11"/>
       <c r="Q40" s="11"/>
     </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="41" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B41" t="s">
         <v>35</v>
       </c>
@@ -4687,7 +4687,7 @@
       <c r="P41" s="11"/>
       <c r="Q41" s="11"/>
     </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="42" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B42" t="s">
         <v>117</v>
       </c>
@@ -4704,7 +4704,7 @@
       <c r="P42" s="11"/>
       <c r="Q42" s="11"/>
     </row>
-    <row r="43" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="43" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B43" t="s">
         <v>111</v>
       </c>
@@ -4721,7 +4721,7 @@
       <c r="P43" s="11"/>
       <c r="Q43" s="11"/>
     </row>
-    <row r="44" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="44" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B44" t="s">
         <v>112</v>
       </c>
@@ -4738,7 +4738,7 @@
       <c r="P44" s="11"/>
       <c r="Q44" s="11"/>
     </row>
-    <row r="45" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="45" spans="2:17" x14ac:dyDescent="0.5">
       <c r="F45" s="11"/>
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
@@ -4752,7 +4752,7 @@
       <c r="P45" s="11"/>
       <c r="Q45" s="11"/>
     </row>
-    <row r="46" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="46" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B46" s="7" t="s">
         <v>36</v>
       </c>
@@ -4769,7 +4769,7 @@
       <c r="P46" s="11"/>
       <c r="Q46" s="11"/>
     </row>
-    <row r="47" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="47" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B47" s="7"/>
       <c r="F47" s="11"/>
       <c r="G47" s="11"/>
@@ -4784,7 +4784,7 @@
       <c r="P47" s="11"/>
       <c r="Q47" s="11"/>
     </row>
-    <row r="48" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="48" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B48" t="s">
         <v>8</v>
       </c>
@@ -4801,7 +4801,7 @@
       <c r="P48" s="11"/>
       <c r="Q48" s="11"/>
     </row>
-    <row r="49" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="49" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B49" t="s">
         <v>37</v>
       </c>
@@ -4818,7 +4818,7 @@
       <c r="P49" s="11"/>
       <c r="Q49" s="11"/>
     </row>
-    <row r="50" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="50" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B50" t="s">
         <v>38</v>
       </c>
@@ -4835,7 +4835,7 @@
       <c r="P50" s="11"/>
       <c r="Q50" s="11"/>
     </row>
-    <row r="51" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="51" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B51" t="s">
         <v>39</v>
       </c>
@@ -4852,7 +4852,7 @@
       <c r="P51" s="11"/>
       <c r="Q51" s="11"/>
     </row>
-    <row r="52" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="52" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B52" t="s">
         <v>40</v>
       </c>
@@ -4869,7 +4869,7 @@
       <c r="P52" s="11"/>
       <c r="Q52" s="11"/>
     </row>
-    <row r="53" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="53" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B53" t="s">
         <v>41</v>
       </c>
@@ -4886,7 +4886,7 @@
       <c r="P53" s="11"/>
       <c r="Q53" s="11"/>
     </row>
-    <row r="54" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="54" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B54" t="s">
         <v>42</v>
       </c>
@@ -4903,7 +4903,7 @@
       <c r="P54" s="11"/>
       <c r="Q54" s="11"/>
     </row>
-    <row r="55" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="55" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B55" t="s">
         <v>43</v>
       </c>
@@ -4920,7 +4920,7 @@
       <c r="P55" s="11"/>
       <c r="Q55" s="11"/>
     </row>
-    <row r="56" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="56" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B56" t="s">
         <v>44</v>
       </c>
@@ -4937,7 +4937,7 @@
       <c r="P56" s="11"/>
       <c r="Q56" s="11"/>
     </row>
-    <row r="57" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="57" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B57" t="s">
         <v>45</v>
       </c>
@@ -4954,7 +4954,7 @@
       <c r="P57" s="11"/>
       <c r="Q57" s="11"/>
     </row>
-    <row r="58" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="58" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B58" t="s">
         <v>46</v>
       </c>
@@ -4971,7 +4971,7 @@
       <c r="P58" s="11"/>
       <c r="Q58" s="11"/>
     </row>
-    <row r="59" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="59" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B59" t="s">
         <v>47</v>
       </c>
@@ -4988,7 +4988,7 @@
       <c r="P59" s="11"/>
       <c r="Q59" s="11"/>
     </row>
-    <row r="60" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="60" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B60" t="s">
         <v>48</v>
       </c>
@@ -5005,7 +5005,7 @@
       <c r="P60" s="11"/>
       <c r="Q60" s="11"/>
     </row>
-    <row r="61" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="61" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B61" t="s">
         <v>49</v>
       </c>
@@ -5022,7 +5022,7 @@
       <c r="P61" s="11"/>
       <c r="Q61" s="11"/>
     </row>
-    <row r="62" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="62" spans="2:17" x14ac:dyDescent="0.5">
       <c r="F62" s="11"/>
       <c r="G62" s="11"/>
       <c r="H62" s="11"/>
@@ -5036,7 +5036,7 @@
       <c r="P62" s="11"/>
       <c r="Q62" s="11"/>
     </row>
-    <row r="63" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="63" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B63" s="7" t="s">
         <v>50</v>
       </c>
@@ -5053,7 +5053,7 @@
       <c r="P63" s="11"/>
       <c r="Q63" s="11"/>
     </row>
-    <row r="64" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="64" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B64" s="7"/>
       <c r="F64" s="11"/>
       <c r="G64" s="11"/>
@@ -5068,7 +5068,7 @@
       <c r="P64" s="11"/>
       <c r="Q64" s="11"/>
     </row>
-    <row r="65" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="65" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B65" t="s">
         <v>8</v>
       </c>
@@ -5085,7 +5085,7 @@
       <c r="P65" s="11"/>
       <c r="Q65" s="11"/>
     </row>
-    <row r="66" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="66" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B66" s="2" t="s">
         <v>51</v>
       </c>
@@ -5102,70 +5102,70 @@
       <c r="P66" s="11"/>
       <c r="Q66" s="11"/>
     </row>
-    <row r="67" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="67" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B67" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="68" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="68" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B68" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="69" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="69" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B69" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="70" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="70" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B70" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="71" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="71" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B71" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="72" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="72" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B72" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="73" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="73" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B73" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="74" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="74" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B74" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="75" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="75" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B75" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="77" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="77" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B77" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="78" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="78" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B78" s="7"/>
     </row>
-    <row r="79" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="79" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B79" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="80" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="80" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B80" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="81" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="81" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B81" s="1" t="s">
         <v>62</v>
       </c>
@@ -5182,32 +5182,32 @@
       <c r="P81" s="11"/>
       <c r="Q81" s="11"/>
     </row>
-    <row r="82" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="82" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B82" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="83" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="83" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B83" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="84" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="84" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B84" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="85" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="85" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B85" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="86" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="86" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B86" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="89" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="89" spans="2:17" x14ac:dyDescent="0.5">
       <c r="F89" s="11"/>
       <c r="G89" s="11"/>
       <c r="H89" s="11"/>
@@ -5245,19 +5245,19 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="3.69140625" customWidth="1"/>
-    <col min="2" max="3" width="30.69140625" customWidth="1"/>
-    <col min="4" max="9" width="8.69140625" customWidth="1"/>
+    <col min="1" max="1" width="3.703125" customWidth="1"/>
+    <col min="2" max="3" width="30.703125" customWidth="1"/>
+    <col min="4" max="9" width="8.703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" s="13" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" s="13" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="B2" s="13" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -5265,7 +5265,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -5273,7 +5273,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -5281,7 +5281,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -5289,7 +5289,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="8" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:3" s="8" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="B14" s="8" t="s">
         <v>72</v>
       </c>
@@ -5297,7 +5297,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B15" t="s">
         <v>74</v>
       </c>
@@ -5319,18 +5319,18 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="3.69140625" customWidth="1"/>
-    <col min="2" max="3" width="30.69140625" customWidth="1"/>
+    <col min="1" max="1" width="3.703125" customWidth="1"/>
+    <col min="2" max="3" width="30.703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" s="13" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" s="13" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="B2" s="13" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -5338,7 +5338,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -5346,7 +5346,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -5354,7 +5354,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -5362,12 +5362,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="10" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="11" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="12" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="13" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="1:3" s="8" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="10" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="11" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="12" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="13" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="14" spans="1:3" s="8" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="B14" s="8" t="s">
         <v>78</v>
       </c>
@@ -5375,7 +5375,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B15" t="s">
         <v>80</v>
       </c>
@@ -5383,7 +5383,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B16" t="s">
         <v>81</v>
       </c>
@@ -5391,7 +5391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B17" t="s">
         <v>82</v>
       </c>
@@ -5414,17 +5414,17 @@
       <selection activeCell="A11" sqref="A11:R35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="3.69140625" customWidth="1"/>
-    <col min="2" max="2" width="19.53515625" customWidth="1"/>
-    <col min="3" max="3" width="10.15234375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.3046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.3828125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="75.15234375" customWidth="1"/>
+    <col min="1" max="1" width="3.703125" customWidth="1"/>
+    <col min="2" max="2" width="19.52734375" customWidth="1"/>
+    <col min="3" max="3" width="10.17578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.29296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.3515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="75.17578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" s="13" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:18" s="13" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="B2" s="13" t="s">
         <v>83</v>
       </c>
@@ -5432,7 +5432,7 @@
       <c r="F2" s="18"/>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.5">
       <c r="C3" s="1"/>
       <c r="F3" s="9"/>
       <c r="G3" s="17"/>
@@ -5448,7 +5448,7 @@
       <c r="Q3" s="11"/>
       <c r="R3" s="11"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -5459,32 +5459,32 @@
       <c r="F4" s="9"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.5">
       <c r="C5" s="1"/>
       <c r="F5" s="9"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.5">
       <c r="C6" s="1"/>
       <c r="F6" s="9"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.5">
       <c r="C7" s="1"/>
       <c r="F7" s="9"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.5">
       <c r="C8" s="1"/>
       <c r="F8" s="9"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.5">
       <c r="C9" s="1"/>
       <c r="F9" s="9"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.5">
       <c r="B10" t="s">
         <v>72</v>
       </c>
@@ -5501,7 +5501,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.5">
       <c r="B11" t="s">
         <v>74</v>
       </c>
@@ -5518,7 +5518,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.5">
       <c r="B12" t="s">
         <v>74</v>
       </c>
@@ -5535,7 +5535,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.5">
       <c r="B13" t="s">
         <v>74</v>
       </c>
@@ -5552,7 +5552,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.5">
       <c r="B14" t="s">
         <v>74</v>
       </c>
@@ -5569,7 +5569,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.5">
       <c r="B15" t="s">
         <v>74</v>
       </c>
@@ -5586,7 +5586,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.5">
       <c r="B16" t="s">
         <v>74</v>
       </c>
@@ -5603,7 +5603,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B17" t="s">
         <v>74</v>
       </c>
@@ -5620,7 +5620,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B18" t="s">
         <v>74</v>
       </c>
@@ -5637,7 +5637,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B19" t="s">
         <v>74</v>
       </c>
@@ -5654,7 +5654,7 @@
         <v>1000011</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B20" t="s">
         <v>74</v>
       </c>
@@ -5671,7 +5671,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B21" t="s">
         <v>74</v>
       </c>
@@ -5688,7 +5688,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B22" t="s">
         <v>74</v>
       </c>
@@ -5705,7 +5705,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B23" t="s">
         <v>74</v>
       </c>
@@ -5722,7 +5722,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B24" t="s">
         <v>74</v>
       </c>
@@ -5739,7 +5739,7 @@
         <v>35.321100000000001</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B25" t="s">
         <v>74</v>
       </c>
@@ -5756,7 +5756,7 @@
         <v>-119.5808</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B26" t="s">
         <v>74</v>
       </c>
@@ -5773,7 +5773,7 @@
         <v>45152</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B27" t="s">
         <v>74</v>
       </c>
@@ -5790,7 +5790,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B28" t="s">
         <v>74</v>
       </c>
@@ -5807,7 +5807,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B29" t="s">
         <v>74</v>
       </c>
@@ -5824,7 +5824,7 @@
         <v>45468</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B30" t="s">
         <v>74</v>
       </c>
@@ -5841,7 +5841,7 @@
         <v>45152</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B31" t="s">
         <v>74</v>
       </c>
@@ -5858,7 +5858,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B32" t="s">
         <v>74</v>
       </c>
@@ -5875,7 +5875,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B33" t="s">
         <v>74</v>
       </c>
@@ -5892,7 +5892,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B34" t="s">
         <v>74</v>
       </c>
@@ -5909,7 +5909,7 @@
         <v>45159.666666666664</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B35" t="s">
         <v>74</v>
       </c>
@@ -5936,17 +5936,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="e20ceb87-0d79-402a-b4b9-75d78589c76d" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -5955,7 +5944,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000E9A34E7C7C736409D4BDE6375CCC276" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0cf521a6d855790dbe6a6d894ff439cd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32" xmlns:ns3="e20ceb87-0d79-402a-b4b9-75d78589c76d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a45aa6d812898c4b0f52b4c3685679ce" ns2:_="" ns3:_="">
     <xsd:import namespace="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32"/>
@@ -6190,18 +6179,18 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{368BC477-8FFD-4C56-8224-F3CCFEFBFA36}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e20ceb87-0d79-402a-b4b9-75d78589c76d"/>
-    <ds:schemaRef ds:uri="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="e20ceb87-0d79-402a-b4b9-75d78589c76d" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{393EEAE4-A9A0-45DD-A8E7-CAAABB0BE8BF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -6209,7 +6198,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{533C6BB5-3BBA-46E5-A63A-38A55F0F20F9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6226,4 +6215,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{368BC477-8FFD-4C56-8224-F3CCFEFBFA36}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e20ceb87-0d79-402a-b4b9-75d78589c76d"/>
+    <ds:schemaRef ds:uri="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>